<commit_message>
SN: TAS update some forms.
</commit_message>
<xml_diff>
--- a/LF/TAS/Senegal/sn_lf_tas_2_partcipants_202101.xlsx
+++ b/LF/TAS/Senegal/sn_lf_tas_2_partcipants_202101.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Senegal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3B2F28-F778-4A1A-B095-3DE7536B15AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BAAF7E-EB60-4961-8956-D522FD89F88D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -317,21 +317,6 @@
     <t>concat(${p_cluster_id},'-',substr(random(),3,9))</t>
   </si>
   <si>
-    <t>. &gt;= 5 and . &lt;= 120</t>
-  </si>
-  <si>
-    <t>The age must be between 5 and 120 years</t>
-  </si>
-  <si>
-    <t>L'age doit être compris entre 5 et 120 ans</t>
-  </si>
-  <si>
-    <t>sn_lf_tas_2_partcipants_202101</t>
-  </si>
-  <si>
-    <t>(Janvier 2021) 2. TAS FL Formulaire Participants</t>
-  </si>
-  <si>
     <t>p_eu_name</t>
   </si>
   <si>
@@ -360,6 +345,21 @@
   </si>
   <si>
     <t>Sélectionner le code de votre école</t>
+  </si>
+  <si>
+    <t>The age must be between 5 and 9 years</t>
+  </si>
+  <si>
+    <t>. &gt;= 5 and . &lt;= 9</t>
+  </si>
+  <si>
+    <t>L'age doit être compris entre 5 et 9 ans</t>
+  </si>
+  <si>
+    <t>sn_lf_tas_2_partcipants_202101_v2</t>
+  </si>
+  <si>
+    <t>(Janvier 2021) 2. TAS FL Formulaire Participants V2</t>
   </si>
 </sst>
 </file>
@@ -873,11 +873,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD10"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -993,14 +993,14 @@
         <v>25</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
@@ -1021,14 +1021,14 @@
         <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12"/>
@@ -1052,11 +1052,11 @@
         <v>92</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
@@ -1080,11 +1080,11 @@
         <v>93</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
@@ -1173,13 +1173,13 @@
       <c r="F9" s="11"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>75</v>
@@ -1554,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C2">
         <v>20210114</v>

</xml_diff>